<commit_message>
Xuất nhập khẩu visualization
</commit_message>
<xml_diff>
--- a/data/xuat_nhap/xk_nk_cctm.xlsx
+++ b/data/xuat_nhap/xk_nk_cctm.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Year 3\HK2\-Visualization-Overview-of-Viet-Nam-socio-economic\data\xuat_nhap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4F5109-83D6-44EB-8852-3ACB914B742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF4EC7D-3397-4318-A216-827142963C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Xuất" sheetId="1" r:id="rId1"/>
-    <sheet name="Nhập" sheetId="4" r:id="rId2"/>
-    <sheet name="XN_CCTM" sheetId="5" r:id="rId3"/>
-    <sheet name="Top_Xuất khẩu" sheetId="9" r:id="rId4"/>
-    <sheet name="Top_XK" sheetId="11" r:id="rId5"/>
-    <sheet name="Top_Nhập khẩu" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
+    <sheet name="Nhập" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId4"/>
+    <sheet name="XN_CCTM" sheetId="5" r:id="rId5"/>
+    <sheet name="Top_Xuất khẩu" sheetId="10" r:id="rId6"/>
+    <sheet name="Top_Nhập khẩu" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="90">
   <si>
     <t>Nhóm/Mặt hàng chủ yếu</t>
   </si>
@@ -307,19 +308,18 @@
     <t>Tháng</t>
   </si>
   <si>
-    <t>XN</t>
+    <t>Mặt hàng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-101042A]mmm\ yy;@"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -352,15 +352,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="7" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -414,12 +438,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -437,165 +485,133 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="29">
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-101042A]mmm\ yy;@"/>
@@ -811,7 +827,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26BF5E49-4869-471F-9BB5-851C01C56415}" name="Table2" displayName="Table2" ref="A1:M47" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26BF5E49-4869-471F-9BB5-851C01C56415}" name="Table2" displayName="Table2" ref="A1:M47" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A1:M47" xr:uid="{26BF5E49-4869-471F-9BB5-851C01C56415}"/>
   <tableColumns count="13">
     <tableColumn id="2" xr3:uid="{79ED4EFB-87B7-401B-9031-73D83A69A9EC}" name="Nhóm/Mặt hàng chủ yếu"/>
@@ -833,123 +849,93 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6081B050-18F2-4280-9223-E2439F4CF43B}" name="Table3" displayName="Table3" ref="A1:M55" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67">
-  <autoFilter ref="A1:M55" xr:uid="{6081B050-18F2-4280-9223-E2439F4CF43B}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{70C64DB7-637F-4BBE-9079-2C9339E12C8D}" name="Nhóm/Mặt hàng chủ yếu"/>
-    <tableColumn id="4" xr3:uid="{F45DA3B1-0A90-419C-A8E5-2680545968B8}" name="Trị giá tháng 1" dataDxfId="66" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{C1A9FAA0-2AF9-429A-BF8F-A9BC498DDD61}" name="Trị giá tháng 2" dataDxfId="65" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{C47BB083-CC4E-473C-85CB-E34F03C2D8FF}" name="Trị giá tháng 3" dataDxfId="64" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{0CCAA130-193F-488F-8BEA-11A417E01B27}" name="Trị giá tháng 4" dataDxfId="63" dataCellStyle="Currency"/>
-    <tableColumn id="12" xr3:uid="{E5266FCE-73F2-4475-ABE9-3DB1180CCB6C}" name="Trị giá tháng 5" dataDxfId="62" dataCellStyle="Currency"/>
-    <tableColumn id="14" xr3:uid="{AACBB9E3-4661-4032-A2E5-F270E9C73FA7}" name="Trị giá tháng 6" dataDxfId="61" dataCellStyle="Currency"/>
-    <tableColumn id="16" xr3:uid="{4D2EABA1-5C88-4A8F-8B46-7B4D66C15A9D}" name="Trị giá tháng 7" dataDxfId="60" dataCellStyle="Currency"/>
-    <tableColumn id="18" xr3:uid="{EC706DDB-718A-4B48-86BA-D705DFEA6F9E}" name="Trị giá tháng 8" dataDxfId="59" dataCellStyle="Currency"/>
-    <tableColumn id="20" xr3:uid="{16134F64-D50B-4C7E-8BE8-D601333FCAF5}" name="Trị giá tháng 9" dataDxfId="58" dataCellStyle="Currency"/>
-    <tableColumn id="22" xr3:uid="{B04E8BC3-E5EA-47FE-AA68-01E23D829F86}" name="Trị giá tháng 10" dataDxfId="57" dataCellStyle="Currency"/>
-    <tableColumn id="24" xr3:uid="{3A66ACD9-6851-49B4-8602-5F2CF3DCB6A2}" name="Trị giá tháng 11" dataDxfId="56" dataCellStyle="Currency"/>
-    <tableColumn id="26" xr3:uid="{EE60E3E4-749D-457F-B58E-52DC24E6E5F9}" name="Trị giá tháng 12" dataDxfId="55" dataCellStyle="Currency"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{443D41B6-9C40-4306-BA81-28F3A1A92C4F}" name="Table4" displayName="Table4" ref="A1:B47" totalsRowShown="0">
+  <autoFilter ref="A1:B47" xr:uid="{443D41B6-9C40-4306-BA81-28F3A1A92C4F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E7106F8E-5F56-4B17-ABB8-6D5AE0DE5761}" name="Mặt hàng" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{56E9782A-21BC-4419-AEBA-ACADA5A86A75}" name="Xuất khẩu" dataDxfId="4" dataCellStyle="Currency">
+      <calculatedColumnFormula>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E937060-2777-4CCB-8D47-1AD6F7317CD7}" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0" dataDxfId="54" dataCellStyle="Currency">
-  <autoFilter ref="A1:D13" xr:uid="{9E937060-2777-4CCB-8D47-1AD6F7317CD7}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{166A7B19-628C-4499-A723-FD483EAA7D72}" name="Xuất khẩu" dataDxfId="53" dataCellStyle="Currency"/>
-    <tableColumn id="2" xr3:uid="{532A81DA-2A01-4B7D-B501-EE05E733677E}" name="Nhập khẩu" dataDxfId="52" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{E5AE6E93-2155-444A-8251-09D60B274F2C}" name="Cán cân thương mại" dataDxfId="51" dataCellStyle="Currency">
-      <calculatedColumnFormula>A2-B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{001CA8FC-1B46-4280-A8BA-21BFA6391253}" name="Tháng" dataDxfId="50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6081B050-18F2-4280-9223-E2439F4CF43B}" name="Table3" displayName="Table3" ref="A1:M55" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="A1:M55" xr:uid="{6081B050-18F2-4280-9223-E2439F4CF43B}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{70C64DB7-637F-4BBE-9079-2C9339E12C8D}" name="Nhóm/Mặt hàng chủ yếu"/>
+    <tableColumn id="4" xr3:uid="{F45DA3B1-0A90-419C-A8E5-2680545968B8}" name="Trị giá tháng 1" dataDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{C1A9FAA0-2AF9-429A-BF8F-A9BC498DDD61}" name="Trị giá tháng 2" dataDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{C47BB083-CC4E-473C-85CB-E34F03C2D8FF}" name="Trị giá tháng 3" dataDxfId="20" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{0CCAA130-193F-488F-8BEA-11A417E01B27}" name="Trị giá tháng 4" dataDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="12" xr3:uid="{E5266FCE-73F2-4475-ABE9-3DB1180CCB6C}" name="Trị giá tháng 5" dataDxfId="18" dataCellStyle="Currency"/>
+    <tableColumn id="14" xr3:uid="{AACBB9E3-4661-4032-A2E5-F270E9C73FA7}" name="Trị giá tháng 6" dataDxfId="17" dataCellStyle="Currency"/>
+    <tableColumn id="16" xr3:uid="{4D2EABA1-5C88-4A8F-8B46-7B4D66C15A9D}" name="Trị giá tháng 7" dataDxfId="16" dataCellStyle="Currency"/>
+    <tableColumn id="18" xr3:uid="{EC706DDB-718A-4B48-86BA-D705DFEA6F9E}" name="Trị giá tháng 8" dataDxfId="15" dataCellStyle="Currency"/>
+    <tableColumn id="20" xr3:uid="{16134F64-D50B-4C7E-8BE8-D601333FCAF5}" name="Trị giá tháng 9" dataDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="22" xr3:uid="{B04E8BC3-E5EA-47FE-AA68-01E23D829F86}" name="Trị giá tháng 10" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="24" xr3:uid="{3A66ACD9-6851-49B4-8602-5F2CF3DCB6A2}" name="Trị giá tháng 11" dataDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="26" xr3:uid="{EE60E3E4-749D-457F-B58E-52DC24E6E5F9}" name="Trị giá tháng 12" dataDxfId="11" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BD1ADBB0-6B68-4927-97C0-2F0D8B015F89}" name="Table7" displayName="Table7" ref="A1:B47" totalsRowShown="0">
-  <autoFilter ref="A1:B47" xr:uid="{BD1ADBB0-6B68-4927-97C0-2F0D8B015F89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E6109B75-592C-4873-B4E9-5398D1567EDC}" name="Table8" displayName="Table8" ref="A1:B53" totalsRowShown="0">
+  <autoFilter ref="A1:B53" xr:uid="{E6109B75-592C-4873-B4E9-5398D1567EDC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A3846FBF-073F-4226-8401-C631D11CD32F}" name="Mặt hàng" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2029476B-98D3-4FB2-B0BF-5514825FF3D8}" name="Nhập khẩu" dataDxfId="1" dataCellStyle="Currency">
+      <calculatedColumnFormula>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E937060-2777-4CCB-8D47-1AD6F7317CD7}" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0" dataDxfId="10" dataCellStyle="Currency">
+  <autoFilter ref="A1:D13" xr:uid="{9E937060-2777-4CCB-8D47-1AD6F7317CD7}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{166A7B19-628C-4499-A723-FD483EAA7D72}" name="Xuất khẩu" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{532A81DA-2A01-4B7D-B501-EE05E733677E}" name="Nhập khẩu" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{E5AE6E93-2155-444A-8251-09D60B274F2C}" name="Cán cân thương mại" dataDxfId="7" dataCellStyle="Currency">
+      <calculatedColumnFormula>A2-B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{001CA8FC-1B46-4280-A8BA-21BFA6391253}" name="Tháng" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{81096C29-46B6-46C8-9056-BE60224665F2}" name="Table6" displayName="Table6" ref="A1:B47" totalsRowShown="0">
+  <autoFilter ref="A1:B47" xr:uid="{81096C29-46B6-46C8-9056-BE60224665F2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B47">
     <sortCondition descending="1" ref="B1:B47"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DD13914-8FE8-47D1-9D02-6B443E4BF203}" name="XN"/>
-    <tableColumn id="5" xr3:uid="{586A103B-8800-4673-A0CD-5EAF879AD9D4}" name="Xuất khẩu" dataDxfId="49" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{CDE4636E-EDD3-4E14-A5C1-E8357BAA1D29}" name="Mặt hàng"/>
+    <tableColumn id="2" xr3:uid="{4CDC1C05-B6D3-4DD4-A837-88D281E1A064}" name="Xuất khẩu" dataDxfId="3" dataCellStyle="Currency"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{61E17410-F3A3-4A95-97C9-D8FF6A189BCF}" name="Table10" displayName="Table10" ref="A1:AU2" totalsRowShown="0" dataDxfId="0" dataCellStyle="Currency">
-  <autoFilter ref="A1:AU2" xr:uid="{61E17410-F3A3-4A95-97C9-D8FF6A189BCF}"/>
-  <tableColumns count="47">
-    <tableColumn id="1" xr3:uid="{A22FC966-842C-4E08-A77D-C3994A0FAB89}" name="XN" dataDxfId="47" dataCellStyle="Currency"/>
-    <tableColumn id="2" xr3:uid="{C0F00A73-DCB6-4C47-88C8-5E300BB9E453}" name="Thức ăn gia súc và nguyên liệu" dataDxfId="46" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{F577090F-D62A-4661-884E-F4F2C08C53D0}" name="Sản phẩm mây, tre, cói và thảm" dataDxfId="45" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{3A12D6E8-9BF3-40C0-9C4F-BCF7F7D20B8E}" name="Phân bón các loại" dataDxfId="44" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{31CC9FE9-4F51-4025-B40D-75EBD7661E2A}" name="Nguyên phụ liệu dệt, may, da, giày" dataDxfId="43" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{211EF2E8-DE94-47CF-8D9E-D2E10CE99E41}" name="Xăng dầu các loại" dataDxfId="42" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{45679181-9815-40DE-BADD-F5AC197BE2BC}" name="Than các loại" dataDxfId="41" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{1590535A-0D3E-4C43-93D2-7B2E10432114}" name="Hóa chất" dataDxfId="40" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{17F5F62B-4F26-4E65-9462-B9E0BDC53390}" name="Đá quý, kim loại quý và sản phẩm" dataDxfId="39" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{45AD08A0-E00C-420A-B4C5-ADB9E64F531A}" name="Máy vi tính, sản phẩm điện tử và linh kiện" dataDxfId="38" dataCellStyle="Currency"/>
-    <tableColumn id="11" xr3:uid="{E15FA1C4-6B81-436C-A673-24268C93B5D4}" name="Thủy tinh và các sản phẩm từ thủy tinh" dataDxfId="37" dataCellStyle="Currency"/>
-    <tableColumn id="12" xr3:uid="{29D94A07-FD37-4F71-8AF5-E1CD62664323}" name="Vải mành, vải kỹ thuật khác" dataDxfId="36" dataCellStyle="Currency"/>
-    <tableColumn id="13" xr3:uid="{9BBF6E4D-C139-4954-BB29-6D72DE6E530E}" name="Điện thoại các loại và linh kiện" dataDxfId="35" dataCellStyle="Currency"/>
-    <tableColumn id="14" xr3:uid="{5F8A00B3-AF9D-4436-B1AE-72E79F6F708B}" name="Kim loại thường khác và sản phẩm" dataDxfId="34" dataCellStyle="Currency"/>
-    <tableColumn id="15" xr3:uid="{397DF167-0086-4024-BBDE-69AE54D2412E}" name="Gỗ và sản phẩm gỗ" dataDxfId="33" dataCellStyle="Currency"/>
-    <tableColumn id="16" xr3:uid="{7D1B65A4-18E4-455E-BCAA-810AAB324A6E}" name="Hàng dệt, may" dataDxfId="32" dataCellStyle="Currency"/>
-    <tableColumn id="17" xr3:uid="{6C6A3E4C-56BF-4D18-B0E2-559BCE5ED4C0}" name="Sắn và các sản phẩm từ sắn" dataDxfId="31" dataCellStyle="Currency"/>
-    <tableColumn id="18" xr3:uid="{03C54046-096A-4640-A175-A87485816F07}" name="Chất dẻo nguyên liệu" dataDxfId="30" dataCellStyle="Currency"/>
-    <tableColumn id="19" xr3:uid="{9C4B459E-5D97-4248-B582-13BAA51C1D2C}" name="Máy móc, thiết bị, dụng cụ phụ tùng khác" dataDxfId="29" dataCellStyle="Currency"/>
-    <tableColumn id="20" xr3:uid="{EB1CA2FF-8FEC-4CD4-A018-57177228C553}" name="Cao su" dataDxfId="28" dataCellStyle="Currency"/>
-    <tableColumn id="21" xr3:uid="{EF0B7C58-33EF-4027-A81F-32BF1A51DD66}" name="Clanhke và xi măng" dataDxfId="27" dataCellStyle="Currency"/>
-    <tableColumn id="22" xr3:uid="{20E4AAA1-DF12-49F1-B146-A2A0A3DD0F57}" name="Quặng và khoáng sản khác" dataDxfId="26" dataCellStyle="Currency"/>
-    <tableColumn id="23" xr3:uid="{E61F5057-B291-49C9-97D6-9D0EBD5A3D1F}" name="Sản phẩm gốm, sứ" dataDxfId="25" dataCellStyle="Currency"/>
-    <tableColumn id="24" xr3:uid="{5AE16AD5-8ED3-417A-9625-25A6EDF44BF0}" name="Đồ chơi, dụng cụ thể thao và bộ phận" dataDxfId="24" dataCellStyle="Currency"/>
-    <tableColumn id="25" xr3:uid="{C8424E32-936B-480C-BDCE-BAEEDFD34CF9}" name="Chè" dataDxfId="23" dataCellStyle="Currency"/>
-    <tableColumn id="26" xr3:uid="{10B94FFE-BF88-4701-9167-B22397DDC95C}" name="Sản phẩm từ sắt thép" dataDxfId="22" dataCellStyle="Currency"/>
-    <tableColumn id="27" xr3:uid="{6B4B7932-2F16-41CA-B090-4D7A70D4F9C4}" name="Xơ, sợi dệt các loại" dataDxfId="21" dataCellStyle="Currency"/>
-    <tableColumn id="28" xr3:uid="{6C635872-EBDF-40D1-A134-B43BB90DF0A6}" name="Túi xách, ví,vali, mũ, ô, dù" dataDxfId="20" dataCellStyle="Currency"/>
-    <tableColumn id="29" xr3:uid="{7950B8A8-6034-45B1-9088-DDB63D0C6CC1}" name="Dầu thô" dataDxfId="19" dataCellStyle="Currency"/>
-    <tableColumn id="30" xr3:uid="{70798E83-0AEB-455C-B6FA-77C5817DDFDC}" name="Sản phẩm hóa chất" dataDxfId="18" dataCellStyle="Currency"/>
-    <tableColumn id="31" xr3:uid="{2F47DC24-28E0-4549-803C-B31E69F2AAE7}" name="Cà phê" dataDxfId="17" dataCellStyle="Currency"/>
-    <tableColumn id="32" xr3:uid="{D7DFC462-2235-41DE-8801-7E18BD7D3B2C}" name="Gạo" dataDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="33" xr3:uid="{C6CCCBB8-26BD-449F-84CE-C102599C2ED1}" name="Hàng hóa khác" dataDxfId="15" dataCellStyle="Currency"/>
-    <tableColumn id="34" xr3:uid="{EF1CDE7C-492E-4682-AC06-864E7EBAC93C}" name="Hàng thủy sản" dataDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="35" xr3:uid="{67E02BDF-CA69-4576-840A-401FDBCA204D}" name="Dây điện và dây cáp điện" dataDxfId="13" dataCellStyle="Currency"/>
-    <tableColumn id="36" xr3:uid="{137B0675-27B0-496E-B978-4A43D3CC7E54}" name="Bánh kẹo và các sản phẩm từ ngũ cốc" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="37" xr3:uid="{A3EBBAC4-7E5E-4D12-A4A2-57232811E416}" name="Phương tiện vận tải và phụ tùng" dataDxfId="11" dataCellStyle="Currency"/>
-    <tableColumn id="38" xr3:uid="{93BCF64B-C142-454E-A6DF-D5F4ACBB59DD}" name="Hàng rau quả" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="39" xr3:uid="{FA8BDF62-CC4B-48E7-9D4C-A5FDBE240C7C}" name="Sắt thép các loại" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="40" xr3:uid="{67406966-3BC8-4107-821F-D74BAAF2A706}" name="Sản phẩm nội thất từ chất liệu khác gỗ" dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="41" xr3:uid="{632BEFDF-DEAF-4C0B-9FAD-13BA4CBDA839}" name="Giấy và các sản phẩm từ giấy" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="42" xr3:uid="{FD56857E-923B-421B-B039-8C3FD9FA818C}" name="Hạt điều" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="43" xr3:uid="{FFE71A1D-D20C-4218-87F0-1E9B5AEFCD12}" name="Hạt tiêu" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="44" xr3:uid="{4E0F8E7F-698F-4392-8E9F-7D2BA16A3E9F}" name="Sản phẩm từ cao su" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="45" xr3:uid="{28CE4D16-D009-4C9D-88DB-18F373862EAD}" name="Giày dép các loại" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="46" xr3:uid="{E87448F1-5601-4459-9FAB-616C221E9FB6}" name="Máy ảnh, máy quay phim và linh kiện" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="47" xr3:uid="{BDDF55FA-159F-464C-B0A1-E1D365429B61}" name="Sản phẩm từ chất dẻo" dataDxfId="1" dataCellStyle="Currency"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BFD096BC-951C-4107-ACBC-D09B24DAC25E}" name="Table710" displayName="Table710" ref="A1:B47" totalsRowShown="0">
-  <autoFilter ref="A1:B47" xr:uid="{BFD096BC-951C-4107-ACBC-D09B24DAC25E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B47">
-    <sortCondition descending="1" ref="B1:B47"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A6E202AB-4B14-42FE-A28E-BA47E159C5D8}" name="Table11" displayName="Table11" ref="A1:B53" totalsRowShown="0">
+  <autoFilter ref="A1:B53" xr:uid="{A6E202AB-4B14-42FE-A28E-BA47E159C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
+    <sortCondition descending="1" ref="B1:B53"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ABF80222-0302-4614-8BBC-BA27FE1D550D}" name="XN"/>
-    <tableColumn id="3" xr3:uid="{412FEE9E-0756-46C0-9CED-42E0E74E824E}" name="Nhập khẩu" dataDxfId="48" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{4E95C906-1DC7-4F7E-9EBA-A6EAA3B7499D}" name="Mặt hàng"/>
+    <tableColumn id="2" xr3:uid="{6929FFF9-DADF-4614-AB14-99FA2382D3FB}" name="Nhập khẩu" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1243,7 +1229,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="A2" sqref="A2:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3189,11 +3175,455 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF11A7A7-4103-4ABD-9FDD-5A1979500DD3}">
+  <dimension ref="A1:B47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>10044842442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>7149055881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4330835314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>5605079397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>256537899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1313747174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>5673125101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1155990061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1229839962</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1038955324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>210582848</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1140438402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>160917225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1731348057</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1930738733</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2804028096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2704748567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>709712938</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2619451076</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>6710133143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3419542989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1226008804</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4227419061</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>803403084</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>16225884847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2092843288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4406071771</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>36965832529</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>771304904</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>22826534970</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2226414069</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>674191339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1185218336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>634303501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>9110221006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4594994034</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4194997744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>72202137652</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>53907272282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>8012187515</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>52097869697</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3491263814</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>14934575381</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3400183385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3746756084</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="12">
+        <f>SUM(Table2[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>18520906460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB6BF0-01DC-45CE-A912-6C02EFBC7AF7}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5522,7 +5952,505 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFD41F8-23B5-4BAF-A58F-AF7A3CC48FAE}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="A1:B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2642727263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1128237094</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2426150655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3219760329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1584921693</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3040094501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1127873795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1384754512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>629117275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1343172386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4900303533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>509643009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2852131188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>7649091205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>8163937386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>8006423410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2044794792</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1693013638</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>8287246052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>7667289916</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>480716564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4381734367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1722000677</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1426699224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>948972735</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>11621698457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>8807682714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3003670146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1082360376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2751715178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2235298066</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1100680357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2887671395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2712503422</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>14882013922</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>7126923878</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1497884738</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>879875782</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>1822797380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>12589405182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>6476731463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>9555946783</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3196749639</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>107062518056</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2228883356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>10387588736</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>2207491112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>48859839079</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3387987539</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>3622020287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>4867040760</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="12">
+        <f>SUM(Table3[[#This Row],[Trị giá tháng 1]:[Trị giá tháng 12]])</f>
+        <v>633073399</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24B0B9B-4C15-4CC1-9908-5F7FC86ECF32}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -5763,12 +6691,412 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70F2179-D5AD-4445-B459-CACCE45FC9E6}">
-  <dimension ref="A1:E47"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F25E587-ECE9-4FED-B3CA-739531198D2B}">
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="12">
+        <v>72202137652</v>
+      </c>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="12">
+        <v>53907272282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="12">
+        <v>52097869697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="12">
+        <v>36965832529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="12">
+        <v>22826534970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="12">
+        <v>18520906460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="12">
+        <v>16225884847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="12">
+        <v>14934575381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="12">
+        <v>10044842442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="12">
+        <v>9110221006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="12">
+        <v>8012187515</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12">
+        <v>7149055881</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="12">
+        <v>6710133143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="12">
+        <v>5673125101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="12">
+        <v>5605079397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="12">
+        <v>4594994034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="12">
+        <v>4406071771</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="12">
+        <v>4330835314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="12">
+        <v>4227419061</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="12">
+        <v>4194997744</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="12">
+        <v>3746756084</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="12">
+        <v>3491263814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="12">
+        <v>3419542989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12">
+        <v>3400183385</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="12">
+        <v>2804028096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="12">
+        <v>2704748567</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="12">
+        <v>2619451076</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2226414069</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="12">
+        <v>2092843288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="12">
+        <v>1930738733</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="12">
+        <v>1731348057</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1313747174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="12">
+        <v>1229839962</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1226008804</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1185218336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1155990061</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="12">
+        <v>1140438402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="12">
+        <v>1038955324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="12">
+        <v>803403084</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="12">
+        <v>771304904</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="12">
+        <v>709712938</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="12">
+        <v>674191339</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="12">
+        <v>634303501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="12">
+        <v>256537899</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="12">
+        <v>210582848</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="12">
+        <v>160917225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70F2179-D5AD-4445-B459-CACCE45FC9E6}">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5784,1165 +7112,465 @@
         <v>89</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B2" s="12">
-        <v>72202137652</v>
+        <v>107062518056</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B3" s="12">
-        <v>53907272282</v>
+        <v>48859839079</v>
       </c>
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B4" s="12">
-        <v>52097869697</v>
+        <v>14882013922</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B5" s="12">
-        <v>36965832529</v>
+        <v>12589405182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6" s="12">
-        <v>22826534970</v>
+        <v>11621698457</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="B7" s="12">
-        <v>18520906460</v>
+        <v>10387588736</v>
       </c>
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B8" s="12">
-        <v>16225884847</v>
+        <v>9555946783</v>
       </c>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B9" s="12">
-        <v>14934575381</v>
+        <v>8807682714</v>
       </c>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B10" s="12">
-        <v>10044842442</v>
+        <v>8287246052</v>
       </c>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B11" s="12">
-        <v>9110221006</v>
+        <v>8163937386</v>
       </c>
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B12" s="12">
-        <v>8012187515</v>
+        <v>8006423410</v>
       </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B13" s="12">
-        <v>7149055881</v>
+        <v>7667289916</v>
       </c>
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B14" s="12">
-        <v>6710133143</v>
+        <v>7649091205</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B15" s="12">
-        <v>5673125101</v>
+        <v>7126923878</v>
       </c>
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B16" s="12">
-        <v>5605079397</v>
+        <v>6476731463</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" s="12">
-        <v>4594994034</v>
+        <v>4900303533</v>
       </c>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B18" s="12">
-        <v>4406071771</v>
+        <v>4867040760</v>
       </c>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B19" s="12">
-        <v>4330835314</v>
+        <v>4381734367</v>
       </c>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B20" s="12">
-        <v>4227419061</v>
+        <v>3622020287</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B21" s="12">
-        <v>4194997744</v>
+        <v>3387987539</v>
       </c>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B22" s="12">
-        <v>3746756084</v>
+        <v>3219760329</v>
       </c>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B23" s="12">
-        <v>3491263814</v>
+        <v>3196749639</v>
       </c>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B24" s="12">
-        <v>3419542989</v>
+        <v>3040094501</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B25" s="12">
-        <v>3400183385</v>
+        <v>3003670146</v>
       </c>
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B26" s="12">
-        <v>2804028096</v>
+        <v>2887671395</v>
       </c>
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B27" s="12">
-        <v>2704748567</v>
+        <v>2852131188</v>
       </c>
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B28" s="12">
-        <v>2619451076</v>
+        <v>2751715178</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B29" s="12">
-        <v>2226414069</v>
+        <v>2712503422</v>
       </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B30" s="12">
-        <v>2092843288</v>
+        <v>2642727263</v>
       </c>
       <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B31" s="12">
-        <v>1930738733</v>
+        <v>2426150655</v>
       </c>
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B32" s="12">
-        <v>1731348057</v>
+        <v>2235298066</v>
       </c>
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B33" s="12">
-        <v>1313747174</v>
+        <v>2228883356</v>
       </c>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B34" s="12">
-        <v>1229839962</v>
+        <v>2207491112</v>
       </c>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B35" s="12">
-        <v>1226008804</v>
+        <v>2044794792</v>
       </c>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B36" s="12">
-        <v>1185218336</v>
+        <v>1822797380</v>
       </c>
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B37" s="12">
-        <v>1155990061</v>
+        <v>1722000677</v>
       </c>
       <c r="E37" s="11"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B38" s="12">
-        <v>1140438402</v>
+        <v>1693013638</v>
       </c>
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B39" s="12">
-        <v>1038955324</v>
+        <v>1584921693</v>
       </c>
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B40" s="12">
-        <v>803403084</v>
+        <v>1497884738</v>
       </c>
       <c r="E40" s="11"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B41" s="12">
-        <v>771304904</v>
+        <v>1426699224</v>
       </c>
       <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B42" s="12">
-        <v>709712938</v>
+        <v>1384754512</v>
       </c>
       <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B43" s="12">
-        <v>674191339</v>
+        <v>1343172386</v>
       </c>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B44" s="12">
-        <v>634303501</v>
+        <v>1128237094</v>
       </c>
       <c r="E44" s="11"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B45" s="12">
-        <v>256537899</v>
+        <v>1127873795</v>
       </c>
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B46" s="12">
-        <v>210582848</v>
+        <v>1100680357</v>
       </c>
       <c r="E46" s="11"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1082360376</v>
+      </c>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="12">
-        <v>160917225</v>
-      </c>
-      <c r="E47" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47D0287-62A2-4D30-902B-51C67B44E4E9}">
-  <dimension ref="A1:AU2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="B48" s="12">
+        <v>948972735</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="12">
+        <v>879875782</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="12">
+        <v>633073399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B51" s="12">
+        <v>629117275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="12">
+        <v>509643009</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="14">
-        <v>72202137652</v>
-      </c>
-      <c r="C2" s="14">
-        <v>53907272282</v>
-      </c>
-      <c r="D2" s="14">
-        <v>52097869697</v>
-      </c>
-      <c r="E2" s="14">
-        <v>36965832529</v>
-      </c>
-      <c r="F2" s="14">
-        <v>22826534970</v>
-      </c>
-      <c r="G2" s="14">
-        <v>18520906460</v>
-      </c>
-      <c r="H2" s="14">
-        <v>16225884847</v>
-      </c>
-      <c r="I2" s="14">
-        <v>14934575381</v>
-      </c>
-      <c r="J2" s="14">
-        <v>10044842442</v>
-      </c>
-      <c r="K2" s="14">
-        <v>9110221006</v>
-      </c>
-      <c r="L2" s="14">
-        <v>8012187515</v>
-      </c>
-      <c r="M2" s="14">
-        <v>7149055881</v>
-      </c>
-      <c r="N2" s="14">
-        <v>6710133143</v>
-      </c>
-      <c r="O2" s="14">
-        <v>5673125101</v>
-      </c>
-      <c r="P2" s="14">
-        <v>5605079397</v>
-      </c>
-      <c r="Q2" s="14">
-        <v>4594994034</v>
-      </c>
-      <c r="R2" s="14">
-        <v>4406071771</v>
-      </c>
-      <c r="S2" s="14">
-        <v>4330835314</v>
-      </c>
-      <c r="T2" s="14">
-        <v>4227419061</v>
-      </c>
-      <c r="U2" s="14">
-        <v>4194997744</v>
-      </c>
-      <c r="V2" s="14">
-        <v>3746756084</v>
-      </c>
-      <c r="W2" s="14">
-        <v>3491263814</v>
-      </c>
-      <c r="X2" s="14">
-        <v>3419542989</v>
-      </c>
-      <c r="Y2" s="14">
-        <v>3400183385</v>
-      </c>
-      <c r="Z2" s="14">
-        <v>2804028096</v>
-      </c>
-      <c r="AA2" s="14">
-        <v>2704748567</v>
-      </c>
-      <c r="AB2" s="14">
-        <v>2619451076</v>
-      </c>
-      <c r="AC2" s="14">
-        <v>2226414069</v>
-      </c>
-      <c r="AD2" s="14">
-        <v>2092843288</v>
-      </c>
-      <c r="AE2" s="14">
-        <v>1930738733</v>
-      </c>
-      <c r="AF2" s="14">
-        <v>1731348057</v>
-      </c>
-      <c r="AG2" s="14">
-        <v>1313747174</v>
-      </c>
-      <c r="AH2" s="14">
-        <v>1229839962</v>
-      </c>
-      <c r="AI2" s="14">
-        <v>1226008804</v>
-      </c>
-      <c r="AJ2" s="14">
-        <v>1185218336</v>
-      </c>
-      <c r="AK2" s="14">
-        <v>1155990061</v>
-      </c>
-      <c r="AL2" s="14">
-        <v>1140438402</v>
-      </c>
-      <c r="AM2" s="14">
-        <v>1038955324</v>
-      </c>
-      <c r="AN2" s="14">
-        <v>803403084</v>
-      </c>
-      <c r="AO2" s="14">
-        <v>771304904</v>
-      </c>
-      <c r="AP2" s="14">
-        <v>709712938</v>
-      </c>
-      <c r="AQ2" s="14">
-        <v>674191339</v>
-      </c>
-      <c r="AR2" s="14">
-        <v>634303501</v>
-      </c>
-      <c r="AS2" s="14">
-        <v>256537899</v>
-      </c>
-      <c r="AT2" s="14">
-        <v>210582848</v>
-      </c>
-      <c r="AU2" s="14">
-        <v>160917225</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F25E587-ECE9-4FED-B3CA-739531198D2B}">
-  <dimension ref="A1:B47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" style="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="12">
-        <v>107062518056</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="12">
-        <v>14882013922</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="12">
-        <v>12589405182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="12">
-        <v>11621698457</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="12">
-        <v>10387588736</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="12">
-        <v>9555946783</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="12">
-        <v>8807682714</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="12">
-        <v>8287246052</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="12">
-        <v>8163937386</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="12">
-        <v>8006423410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="12">
-        <v>7667289916</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="12">
-        <v>7649091205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="12">
-        <v>7126923878</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="12">
-        <v>6476731463</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="12">
-        <v>4900303533</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="12">
-        <v>4381734367</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="12">
-        <v>3219760329</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="12">
-        <v>3196749639</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="12">
-        <v>3040094501</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="12">
-        <v>3003670146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="12">
-        <v>2887671395</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="12">
-        <v>2852131188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="12">
-        <v>2751715178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="12">
-        <v>2712503422</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="12">
-        <v>2642727263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="12">
-        <v>2426150655</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="12">
-        <v>2235298066</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="12">
-        <v>2228883356</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="12">
-        <v>2044794792</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="12">
-        <v>1822797380</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="12">
-        <v>1722000677</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="12">
-        <v>1693013638</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="12">
-        <v>1584921693</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="12">
-        <v>1497884738</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="12">
-        <v>1426699224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="12">
-        <v>1384754512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="12">
-        <v>1343172386</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="12">
-        <v>1128237094</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="12">
-        <v>1127873795</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="12">
-        <v>1100680357</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="12">
-        <v>1082360376</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="12">
-        <v>948972735</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="12">
-        <v>879875782</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="12">
-        <v>629117275</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="12">
-        <v>509643009</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="12">
+      <c r="B53" s="12">
         <v>480716564</v>
       </c>
     </row>

</xml_diff>